<commit_message>
new data, adjusted template to match
</commit_message>
<xml_diff>
--- a/nes-lter-doc-transect-info.xlsx
+++ b/nes-lter-doc-transect-info.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20390"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\vscode\nes-lter-doc-transect\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DCD22-3700-479F-B643-ECE9BAC38338}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18198" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="ColumnHeaders"/>
-    <sheet r:id="rId2" sheetId="2" name="CategoricalVariables"/>
-    <sheet r:id="rId3" sheetId="3" name="Personnel"/>
-    <sheet r:id="rId4" sheetId="4" name="Keywords"/>
-    <sheet r:id="rId5" sheetId="5" name="CustomUnits"/>
+    <sheet name="ColumnHeaders" sheetId="6" r:id="rId1"/>
+    <sheet name="CategoricalVariables" sheetId="2" r:id="rId2"/>
+    <sheet name="Personnel" sheetId="3" r:id="rId3"/>
+    <sheet name="Keywords" sheetId="4" r:id="rId4"/>
+    <sheet name="CustomUnits" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
   <si>
     <t>id</t>
   </si>
@@ -197,12 +203,6 @@
     <t>definition</t>
   </si>
   <si>
-    <t>cast type</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>(placeholder)</t>
   </si>
   <si>
@@ -311,9 +311,6 @@
     <t>Lowercase letter indicating replicate subsample drawn from the same rosette bottle</t>
   </si>
   <si>
-    <t>date run</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -323,12 +320,6 @@
     <t>filename</t>
   </si>
   <si>
-    <t>npoc(um)</t>
-  </si>
-  <si>
-    <t>tn(um)</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -365,14 +356,31 @@
     <t>(placeholder; also should be categorical)</t>
   </si>
   <si>
-    <t>distance_km</t>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>npoc</t>
+  </si>
+  <si>
+    <t>tn</t>
+  </si>
+  <si>
+    <t>quality_flag</t>
+  </si>
+  <si>
+    <t>station_distance</t>
+  </si>
+  <si>
+    <t>date_analyzed</t>
+  </si>
+  <si>
+    <t>(placeholder; should it be categorical?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,53 +430,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -479,10 +489,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -520,71 +530,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -612,7 +622,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -635,11 +645,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -648,13 +658,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -664,7 +674,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -673,7 +683,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -682,7 +692,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -690,10 +700,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -758,351 +768,367 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF578CB0-35FB-430E-8661-39A2778CD1E9}">
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" style="8" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="62.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="49.15625" customWidth="1"/>
+    <col min="3" max="3" width="11.3671875" customWidth="1"/>
+    <col min="4" max="4" width="22.9453125" customWidth="1"/>
+    <col min="5" max="5" width="24.3671875" customWidth="1"/>
+    <col min="6" max="6" width="19.05078125" customWidth="1"/>
+    <col min="7" max="7" width="27.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="47.25" customFormat="1" s="5">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33.75" customFormat="1" s="5">
-      <c r="A2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="5">
-      <c r="A3" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="5">
-      <c r="A4" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="5">
-      <c r="A5" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>98</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="F5" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33.75" customFormat="1" s="5">
-      <c r="A6" s="6" t="s">
-        <v>95</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>101</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="5">
-      <c r="A7" s="6" t="s">
-        <v>97</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>104</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>99</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="5">
-      <c r="A8" s="6" t="s">
-        <v>100</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>106</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="31.5" customFormat="1" s="5">
-      <c r="A9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="31.5" customFormat="1" s="5">
-      <c r="A10" s="6" t="s">
-        <v>102</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>93</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="33.75" customFormat="1" s="5">
-      <c r="A11" s="6" t="s">
-        <v>103</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>111</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
-        <v>105</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6"/>
       <c r="F11" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="5">
-      <c r="A12" s="6" t="s">
-        <v>106</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>112</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="5">
-      <c r="A13" s="6" t="s">
+      <c r="F13" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="33.75" customFormat="1" s="5">
-      <c r="A14" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>112</v>
-      </c>
       <c r="C14" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>113</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="5">
-      <c r="A15" s="6" t="s">
-        <v>63</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>114</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="5">
-      <c r="A16" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
         <v>115</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="F16" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1111,22 +1137,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="13.578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -1137,158 +1163,169 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1297,7 +1334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1305,21 +1342,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" style="3" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="24.734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13.578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1351,7 +1382,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -1383,7 +1414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -1415,7 +1446,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1441,7 +1472,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1469,7 +1500,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -1497,7 +1528,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1533,21 +1564,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="5">
+    <row r="1" spans="1:2" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1555,7 +1586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="5">
+    <row r="2" spans="1:2" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1563,7 +1594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="5">
+    <row r="3" spans="1:2" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1571,43 +1602,43 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="5">
+    <row r="10" spans="1:2" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -1619,7 +1650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1627,16 +1658,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" style="3" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="25.26171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1653,7 +1683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1664,7 +1694,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
renamed columns -> doc, dtn
</commit_message>
<xml_diff>
--- a/nes-lter-doc-transect-info.xlsx
+++ b/nes-lter-doc-transect-info.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20390"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\vscode\nes-lter-doc-transect\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DCD22-3700-479F-B643-ECE9BAC38338}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18198" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ColumnHeaders" sheetId="6" r:id="rId1"/>
-    <sheet name="CategoricalVariables" sheetId="2" r:id="rId2"/>
-    <sheet name="Personnel" sheetId="3" r:id="rId3"/>
-    <sheet name="Keywords" sheetId="4" r:id="rId4"/>
-    <sheet name="CustomUnits" sheetId="5" r:id="rId5"/>
+    <sheet r:id="rId1" sheetId="1" name="ColumnHeaders"/>
+    <sheet r:id="rId2" sheetId="2" name="CategoricalVariables"/>
+    <sheet r:id="rId3" sheetId="3" name="Personnel"/>
+    <sheet r:id="rId4" sheetId="4" name="Keywords"/>
+    <sheet r:id="rId5" sheetId="5" name="CustomUnits"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -203,6 +197,12 @@
     <t>definition</t>
   </si>
   <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>cast</t>
+  </si>
+  <si>
     <t>(placeholder)</t>
   </si>
   <si>
@@ -251,6 +251,9 @@
     <t>MVCO</t>
   </si>
   <si>
+    <t>quality_flag</t>
+  </si>
+  <si>
     <t>attributeDefinition</t>
   </si>
   <si>
@@ -284,104 +287,96 @@
     <t>Missing value</t>
   </si>
   <si>
+    <t>CTD rosette cast number chronological per cruise</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>niskin</t>
+  </si>
+  <si>
+    <t>Rosette bottle position number</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date and time in UTC when rosette bottle closed</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>Ship's latitude when rosette bottle closed</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>Ship's longitude when rosette bottle closed</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>Depth of sample below sea surface http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
     <t>categorical</t>
   </si>
   <si>
-    <t>cast</t>
-  </si>
-  <si>
-    <t>CTD rosette cast number chronological per cruise</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>niskin</t>
-  </si>
-  <si>
-    <t>Rosette bottle position number</t>
-  </si>
-  <si>
     <t>replicate</t>
   </si>
   <si>
     <t>Lowercase letter indicating replicate subsample drawn from the same rosette bottle</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>doc</t>
+  </si>
+  <si>
+    <t>dtn</t>
+  </si>
+  <si>
+    <t>(placeholder; should it be categorical?)</t>
+  </si>
+  <si>
+    <t>(placeholder; also should be categorical)</t>
+  </si>
+  <si>
+    <t>station_distance</t>
+  </si>
+  <si>
+    <t>date_analyzed</t>
   </si>
   <si>
     <t>YYYY-MM-DD</t>
   </si>
   <si>
     <t>filename</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Date and time in UTC when rosette bottle closed</t>
-  </si>
-  <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>Ship's latitude when rosette bottle closed</t>
-  </si>
-  <si>
-    <t>degree</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>Ship's longitude when rosette bottle closed</t>
-  </si>
-  <si>
-    <t>depth</t>
-  </si>
-  <si>
-    <t>Depth of sample below sea surface http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
-  </si>
-  <si>
-    <t>meter</t>
-  </si>
-  <si>
-    <t>(placeholder; also should be categorical)</t>
-  </si>
-  <si>
-    <t>sample_type</t>
-  </si>
-  <si>
-    <t>npoc</t>
-  </si>
-  <si>
-    <t>tn</t>
-  </si>
-  <si>
-    <t>quality_flag</t>
-  </si>
-  <si>
-    <t>station_distance</t>
-  </si>
-  <si>
-    <t>date_analyzed</t>
-  </si>
-  <si>
-    <t>(placeholder; should it be categorical?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,6 +387,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -430,55 +431,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="18">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -489,10 +503,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -530,71 +544,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -622,7 +636,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -645,11 +659,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -658,13 +672,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -674,7 +688,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -683,7 +697,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -692,7 +706,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -700,10 +714,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -768,367 +782,370 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF578CB0-35FB-430E-8661-39A2778CD1E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="49.15625" customWidth="1"/>
-    <col min="3" max="3" width="11.3671875" customWidth="1"/>
-    <col min="4" max="4" width="22.9453125" customWidth="1"/>
-    <col min="5" max="5" width="24.3671875" customWidth="1"/>
-    <col min="6" max="6" width="19.05078125" customWidth="1"/>
-    <col min="7" max="7" width="27.3125" customWidth="1"/>
+    <col min="1" max="1" style="3" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="49.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="24.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="27.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="5">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33.75" customFormat="1" s="5">
+      <c r="A2" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
         <v>87</v>
       </c>
+      <c r="G2" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A3" s="16" t="s">
+        <v>60</v>
+      </c>
       <c r="B3" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>98</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A5" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A6" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>104</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A7" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>106</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33.75" customFormat="1" s="5">
+      <c r="A8" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>110</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A9" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33.75" customFormat="1" s="5">
+      <c r="A10" s="16" t="s">
+        <v>107</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>111</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A11" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>112</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A12" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A13" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A14" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>114</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="31.5" customFormat="1" s="5">
+      <c r="A15" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>115</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A16" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>97</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="5">
+      <c r="A17" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1137,195 +1154,195 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="13.578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>60</v>
+      <c r="B3" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="14">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1334,7 +1351,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1342,15 +1359,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="13.578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1382,7 +1405,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -1414,7 +1437,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -1446,7 +1469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1472,7 +1495,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1500,7 +1523,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -1528,7 +1551,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1564,7 +1587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1572,13 +1595,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="8" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1586,7 +1609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1594,7 +1617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1602,43 +1625,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:2" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="5">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -1650,7 +1673,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1658,15 +1681,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.26171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1683,7 +1707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +1718,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
new v2 data table and metadata updates
</commit_message>
<xml_diff>
--- a/nes-lter-doc-transect-info.xlsx
+++ b/nes-lter-doc-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-doc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B578227-97AD-4AA4-AB4D-7541C8944C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D91A88-E805-4FA5-80C0-42F429F7E69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33885" yWindow="4335" windowWidth="21600" windowHeight="12675" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4548" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -416,16 +416,16 @@
     <t>missing data</t>
   </si>
   <si>
-    <t>iode_quality_flag_C</t>
-  </si>
-  <si>
-    <t>iode_quality_flag_N</t>
-  </si>
-  <si>
     <t>IODE Quality Flag primary level for DOC</t>
   </si>
   <si>
     <t>IODE Quality Flag primary level for DTN</t>
+  </si>
+  <si>
+    <t>iode_quality_flag_c</t>
+  </si>
+  <si>
+    <t>iode_quality_flag_n</t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" t="s">
         <v>126</v>
-      </c>
-      <c r="B13" t="s">
-        <v>128</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>92</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" t="s">
         <v>127</v>
-      </c>
-      <c r="B14" t="s">
-        <v>129</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>92</v>
@@ -1242,8 +1242,8 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B20">
         <v>9</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B25">
         <v>9</v>
@@ -1802,7 +1802,7 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add missing row, fix date format, edit methods
</commit_message>
<xml_diff>
--- a/nes-lter-doc-transect-info.xlsx
+++ b/nes-lter-doc-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-doc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D91A88-E805-4FA5-80C0-42F429F7E69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EF2DF1-6B5C-4CD4-906B-F513909D24CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-4548" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4548" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -257,9 +257,6 @@
     <t>character</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>Missing value</t>
   </si>
   <si>
@@ -426,6 +423,9 @@
   </si>
   <si>
     <t>iode_quality_flag_n</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -856,8 +856,8 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,10 +907,10 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -918,125 +918,125 @@
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1044,26 +1044,26 @@
         <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>72</v>
@@ -1071,82 +1071,82 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
-      <c r="F13"/>
+      <c r="F13" s="2"/>
       <c r="G13"/>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
-      <c r="F14"/>
+      <c r="F14" s="2"/>
       <c r="G14"/>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>72</v>
@@ -1162,60 +1162,60 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>72</v>
@@ -1223,10 +1223,10 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1242,7 +1242,7 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:A20"/>
     </sheetView>
   </sheetViews>
@@ -1273,7 +1273,7 @@
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1284,7 +1284,7 @@
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1421,112 +1421,112 @@
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B25">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1687,7 +1687,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -1716,7 +1716,7 @@
         <v>39</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -1748,7 +1748,7 @@
         <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H7" t="s">
         <v>24</v>
@@ -1762,22 +1762,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
         <v>112</v>
-      </c>
-      <c r="C8" t="s">
-        <v>113</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="G8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s">
         <v>24</v>
@@ -1833,7 +1833,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1841,7 +1841,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1849,15 +1849,15 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1865,7 +1865,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
incorporate updated data table, adjust missing value codes
</commit_message>
<xml_diff>
--- a/nes-lter-doc-transect-info.xlsx
+++ b/nes-lter-doc-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-doc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EF2DF1-6B5C-4CD4-906B-F513909D24CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EC0B0E-D1BC-40A9-94E7-F8936A128938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-4548" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27480" yWindow="-3876" windowWidth="18456" windowHeight="12984" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
   <si>
     <t>micromolePerLiter</t>
   </si>
@@ -125,9 +125,6 @@
     <t>NSF</t>
   </si>
   <si>
-    <t>OCE-1655686</t>
-  </si>
-  <si>
     <t>PI</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>character</t>
   </si>
   <si>
-    <t>Missing value</t>
-  </si>
-  <si>
     <t>CTD rosette cast number chronological per cruise</t>
   </si>
   <si>
@@ -275,9 +269,6 @@
     <t>Rosette bottle position number</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>Date and time in UTC when rosette bottle closed</t>
   </si>
   <si>
@@ -371,24 +362,9 @@
     <t>total dissolved nitrogen</t>
   </si>
   <si>
-    <t>Kate</t>
-  </si>
-  <si>
-    <t>Morkeski</t>
-  </si>
-  <si>
-    <t>kmorkeski@whoi.edu</t>
-  </si>
-  <si>
-    <t>0000-0002-2903-5851</t>
-  </si>
-  <si>
     <t>Software Developer</t>
   </si>
   <si>
-    <t>Metadata Provider</t>
-  </si>
-  <si>
     <t>Identifier for water column samples versus acidified MilliQ blanks</t>
   </si>
   <si>
@@ -425,14 +401,41 @@
     <t>iode_quality_flag_n</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>date_time_utc</t>
+  </si>
+  <si>
+    <t>OCE-2322676</t>
+  </si>
+  <si>
+    <t>OCE-2322677</t>
+  </si>
+  <si>
+    <t>OCE-2322678</t>
+  </si>
+  <si>
+    <t>OCE-2322679</t>
+  </si>
+  <si>
+    <t>OCE-2322680</t>
+  </si>
+  <si>
+    <t>OCE-2322681</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +477,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -856,16 +865,16 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
     <col min="2" max="2" width="60.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="24.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.33203125" style="4" bestFit="1" customWidth="1"/>
@@ -873,261 +882,249 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -1136,13 +1133,13 @@
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -1151,83 +1148,71 @@
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>73</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1256,277 +1241,277 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" t="s">
         <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B25">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1539,10 +1524,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,7 +1599,7 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1637,7 +1622,7 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
         <v>24</v>
@@ -1646,22 +1631,22 @@
         <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
         <v>24</v>
@@ -1670,24 +1655,24 @@
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -1699,24 +1684,24 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -1728,27 +1713,27 @@
         <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
         <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="G7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H7" t="s">
         <v>24</v>
@@ -1757,39 +1742,11 @@
         <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G8" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
@@ -1833,7 +1790,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1841,7 +1798,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1849,15 +1806,15 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1865,7 +1822,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
data and metadata updates for v3
</commit_message>
<xml_diff>
--- a/nes-lter-doc-transect-info.xlsx
+++ b/nes-lter-doc-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-doc-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-doc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EC0B0E-D1BC-40A9-94E7-F8936A128938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55DD009-EEEF-423F-BC58-209EDD7014EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27480" yWindow="-3876" windowWidth="18456" windowHeight="12984" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34110" yWindow="2235" windowWidth="14265" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -347,9 +347,6 @@
     <t>water sample from Niskin bottle</t>
   </si>
   <si>
-    <t>Date of laboratory sample analysis</t>
-  </si>
-  <si>
     <t>kilometer</t>
   </si>
   <si>
@@ -429,6 +426,9 @@
   </si>
   <si>
     <t>OCE-2322681</t>
+  </si>
+  <si>
+    <t>Date of laboratory sample analysis (Kujawinski lab) or date data received (Carlson lab)</t>
   </si>
 </sst>
 </file>
@@ -865,14 +865,14 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="60.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="24.44140625" style="4" bestFit="1" customWidth="1"/>
@@ -933,10 +933,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -954,15 +954,15 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>77</v>
@@ -975,10 +975,10 @@
         <v>79</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -996,10 +996,10 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1017,10 +1017,10 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1038,10 +1038,10 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1049,7 +1049,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>88</v>
@@ -1089,10 +1089,10 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
@@ -1110,18 +1110,18 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>88</v>
@@ -1133,10 +1133,10 @@
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>88</v>
@@ -1172,14 +1172,14 @@
         <v>73</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1187,7 +1187,7 @@
         <v>94</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>78</v>
@@ -1204,7 +1204,7 @@
         <v>96</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>71</v>
@@ -1228,7 +1228,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A20"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1269,7 +1269,7 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1406,7 +1406,7 @@
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1417,51 +1417,51 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1472,46 +1472,46 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1526,7 +1526,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1599,7 +1599,7 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1631,7 +1631,7 @@
         <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1655,7 +1655,7 @@
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1672,7 +1672,7 @@
         <v>35</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -1684,7 +1684,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1701,7 +1701,7 @@
         <v>38</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -1713,7 +1713,7 @@
         <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1733,7 +1733,7 @@
         <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H7" t="s">
         <v>24</v>
@@ -1742,7 +1742,7 @@
         <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1790,7 +1790,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1798,7 +1798,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1806,15 +1806,15 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1822,7 +1822,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
move name to middle initial field
</commit_message>
<xml_diff>
--- a/nes-lter-doc-transect-info.xlsx
+++ b/nes-lter-doc-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-doc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55DD009-EEEF-423F-BC58-209EDD7014EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51094AE-F5E8-4782-AA3B-F9B2C97C4D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34110" yWindow="2235" windowWidth="14265" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31560" yWindow="570" windowWidth="21240" windowHeight="13275" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="132">
   <si>
     <t>micromolePerLiter</t>
   </si>
@@ -137,9 +137,6 @@
     <t>contact</t>
   </si>
   <si>
-    <t>E. Taylor</t>
-  </si>
-  <si>
     <t>Crockford</t>
   </si>
   <si>
@@ -429,6 +426,12 @@
   </si>
   <si>
     <t>Date of laboratory sample analysis (Kujawinski lab) or date data received (Carlson lab)</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>E.</t>
   </si>
 </sst>
 </file>
@@ -865,7 +868,7 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -882,36 +885,36 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -920,139 +923,139 @@
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1061,13 +1064,13 @@
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1076,55 +1079,55 @@
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -1133,13 +1136,13 @@
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -1148,13 +1151,13 @@
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1163,51 +1166,51 @@
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1241,277 +1244,277 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" t="s">
         <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1526,8 +1529,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1599,7 +1602,7 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1631,7 +1634,7 @@
         <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1655,24 +1658,27 @@
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -1684,24 +1690,24 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -1713,27 +1719,27 @@
         <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H7" t="s">
         <v>24</v>
@@ -1742,7 +1748,7 @@
         <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1790,7 +1796,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1798,7 +1804,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1806,15 +1812,15 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1822,7 +1828,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add JK, update nutrient citation
</commit_message>
<xml_diff>
--- a/nes-lter-doc-transect-info.xlsx
+++ b/nes-lter-doc-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-doc-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51094AE-F5E8-4782-AA3B-F9B2C97C4D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4190C2C-E652-4F40-98E3-718E24FD9205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31560" yWindow="570" windowWidth="21240" windowHeight="13275" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="136">
   <si>
     <t>micromolePerLiter</t>
   </si>
@@ -432,13 +432,25 @@
   </si>
   <si>
     <t>E.</t>
+  </si>
+  <si>
+    <t>Joanne</t>
+  </si>
+  <si>
+    <t>Koch</t>
+  </si>
+  <si>
+    <t>jkoch@whoi.edu</t>
+  </si>
+  <si>
+    <t>softwareDeveloper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +502,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -515,10 +535,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -561,8 +582,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1527,10 +1550,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1751,10 +1774,40 @@
         <v>128</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{36EE3611-7DB4-4CA8-BA6A-277521B94262}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>